<commit_message>
Primera resolución parcial de FECHAFIN en covid subestudy respond wp2.
</commit_message>
<xml_diff>
--- a/dat/variable_list-EcS_v3.xlsx
+++ b/dat/variable_list-EcS_v3.xlsx
@@ -16,7 +16,7 @@
     <sheet name="EcS-free format" sheetId="1" r:id="rId2"/>
     <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2020,8 +2020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G350"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A339" workbookViewId="0">
-      <selection activeCell="E362" sqref="E362"/>
+    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
+      <selection activeCell="C231" sqref="C231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6517,9 +6517,6 @@
       </c>
       <c r="B225" t="s">
         <v>7</v>
-      </c>
-      <c r="C225">
-        <v>1</v>
       </c>
       <c r="D225" t="s">
         <v>281</v>

</xml_diff>

<commit_message>
deletes unnecessary variable that was miscoded
</commit_message>
<xml_diff>
--- a/dat/variable_list-EcS_v3.xlsx
+++ b/dat/variable_list-EcS_v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cris\Documents\Workspace\respond-wp2-ecs\dat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2FC9FD5-C74E-4FF9-9E96-FA94CFD5FB26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016B111C-CAAA-4307-8AF6-D3EC050D17FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3432" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3422" uniqueCount="487">
   <si>
     <t>label</t>
   </si>
@@ -1707,8 +1707,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:G346" totalsRowShown="0">
-  <autoFilter ref="A1:G346" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:G344" totalsRowShown="0">
+  <autoFilter ref="A1:G344" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="label"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="study"/>
@@ -2019,10 +2019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G346"/>
+  <dimension ref="A1:G344"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="H176" sqref="H176"/>
+      <selection activeCell="I170" sqref="I170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5497,39 +5497,39 @@
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A174" t="s">
+      <c r="A174" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="B174" t="s">
-        <v>7</v>
-      </c>
-      <c r="C174">
-        <v>1</v>
-      </c>
-      <c r="D174" t="s">
-        <v>233</v>
-      </c>
-      <c r="E174" t="s">
+      <c r="B174" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C174" s="3">
+        <v>2</v>
+      </c>
+      <c r="D174" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="E174" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F174" t="s">
-        <v>416</v>
+        <v>469</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A175" s="3" t="s">
+      <c r="A175" t="s">
         <v>213</v>
       </c>
-      <c r="B175" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C175" s="3">
-        <v>2</v>
-      </c>
-      <c r="D175" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="E175" s="3" t="s">
+      <c r="B175" t="s">
+        <v>7</v>
+      </c>
+      <c r="C175">
+        <v>2</v>
+      </c>
+      <c r="D175" t="s">
+        <v>234</v>
+      </c>
+      <c r="E175" t="s">
         <v>15</v>
       </c>
       <c r="F175" t="s">
@@ -5547,7 +5547,7 @@
         <v>2</v>
       </c>
       <c r="D176" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E176" t="s">
         <v>15</v>
@@ -5567,7 +5567,7 @@
         <v>2</v>
       </c>
       <c r="D177" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E177" t="s">
         <v>15</v>
@@ -5587,7 +5587,7 @@
         <v>2</v>
       </c>
       <c r="D178" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E178" t="s">
         <v>15</v>
@@ -5607,7 +5607,7 @@
         <v>2</v>
       </c>
       <c r="D179" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E179" t="s">
         <v>15</v>
@@ -5617,39 +5617,39 @@
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A180" t="s">
-        <v>213</v>
-      </c>
-      <c r="B180" t="s">
-        <v>7</v>
-      </c>
-      <c r="C180">
-        <v>2</v>
-      </c>
-      <c r="D180" t="s">
-        <v>238</v>
-      </c>
-      <c r="E180" t="s">
+      <c r="A180" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C180" s="3">
+        <v>1</v>
+      </c>
+      <c r="D180" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E180" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F180" t="s">
-        <v>469</v>
+        <v>416</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A181" s="3" t="s">
+      <c r="A181" t="s">
         <v>239</v>
       </c>
-      <c r="B181" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C181" s="3">
-        <v>1</v>
-      </c>
-      <c r="D181" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="E181" s="3" t="s">
+      <c r="B181" t="s">
+        <v>7</v>
+      </c>
+      <c r="C181">
+        <v>1</v>
+      </c>
+      <c r="D181" t="s">
+        <v>241</v>
+      </c>
+      <c r="E181" t="s">
         <v>15</v>
       </c>
       <c r="F181" t="s">
@@ -5667,7 +5667,7 @@
         <v>1</v>
       </c>
       <c r="D182" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="E182" t="s">
         <v>15</v>
@@ -5687,7 +5687,7 @@
         <v>1</v>
       </c>
       <c r="D183" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="E183" t="s">
         <v>15</v>
@@ -5707,7 +5707,7 @@
         <v>1</v>
       </c>
       <c r="D184" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="E184" t="s">
         <v>15</v>
@@ -5727,7 +5727,7 @@
         <v>1</v>
       </c>
       <c r="D185" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="E185" t="s">
         <v>15</v>
@@ -5747,7 +5747,7 @@
         <v>1</v>
       </c>
       <c r="D186" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="E186" t="s">
         <v>15</v>
@@ -5757,23 +5757,23 @@
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A187" t="s">
+      <c r="A187" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="B187" t="s">
-        <v>7</v>
-      </c>
-      <c r="C187">
-        <v>1</v>
-      </c>
-      <c r="D187" t="s">
-        <v>245</v>
-      </c>
-      <c r="E187" t="s">
+      <c r="B187" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C187" s="3">
+        <v>2</v>
+      </c>
+      <c r="D187" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E187" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F187" t="s">
-        <v>416</v>
+        <v>469</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.3">
@@ -5784,32 +5784,32 @@
         <v>7</v>
       </c>
       <c r="C188">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D188" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E188" t="s">
         <v>15</v>
       </c>
       <c r="F188" t="s">
-        <v>416</v>
+        <v>469</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A189" s="3" t="s">
+      <c r="A189" t="s">
         <v>239</v>
       </c>
-      <c r="B189" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C189" s="3">
-        <v>2</v>
-      </c>
-      <c r="D189" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="E189" s="3" t="s">
+      <c r="B189" t="s">
+        <v>7</v>
+      </c>
+      <c r="C189">
+        <v>2</v>
+      </c>
+      <c r="D189" t="s">
+        <v>248</v>
+      </c>
+      <c r="E189" t="s">
         <v>15</v>
       </c>
       <c r="F189" t="s">
@@ -5817,62 +5817,62 @@
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A190" t="s">
-        <v>239</v>
-      </c>
-      <c r="B190" t="s">
-        <v>7</v>
-      </c>
-      <c r="C190">
-        <v>2</v>
-      </c>
-      <c r="D190" t="s">
-        <v>247</v>
-      </c>
-      <c r="E190" t="s">
-        <v>15</v>
-      </c>
-      <c r="F190" t="s">
-        <v>469</v>
+      <c r="A190" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C190" s="3">
+        <v>1</v>
+      </c>
+      <c r="D190" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="E190" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F190" s="3" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="B191" t="s">
         <v>7</v>
       </c>
       <c r="C191">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D191" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E191" t="s">
         <v>15</v>
       </c>
       <c r="F191" t="s">
-        <v>469</v>
+        <v>416</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A192" s="3" t="s">
+      <c r="A192" t="s">
         <v>249</v>
       </c>
-      <c r="B192" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C192" s="3">
-        <v>1</v>
-      </c>
-      <c r="D192" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="E192" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F192" s="3" t="s">
+      <c r="B192" t="s">
+        <v>7</v>
+      </c>
+      <c r="C192">
+        <v>1</v>
+      </c>
+      <c r="D192" t="s">
+        <v>252</v>
+      </c>
+      <c r="E192" t="s">
+        <v>15</v>
+      </c>
+      <c r="F192" t="s">
         <v>416</v>
       </c>
     </row>
@@ -5887,7 +5887,7 @@
         <v>1</v>
       </c>
       <c r="D193" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E193" t="s">
         <v>15</v>
@@ -5907,7 +5907,7 @@
         <v>1</v>
       </c>
       <c r="D194" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="E194" t="s">
         <v>15</v>
@@ -5927,7 +5927,7 @@
         <v>1</v>
       </c>
       <c r="D195" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E195" t="s">
         <v>15</v>
@@ -5947,7 +5947,7 @@
         <v>1</v>
       </c>
       <c r="D196" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E196" t="s">
         <v>15</v>
@@ -5967,7 +5967,7 @@
         <v>1</v>
       </c>
       <c r="D197" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E197" t="s">
         <v>15</v>
@@ -5987,7 +5987,7 @@
         <v>1</v>
       </c>
       <c r="D198" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E198" t="s">
         <v>15</v>
@@ -6007,7 +6007,7 @@
         <v>1</v>
       </c>
       <c r="D199" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E199" t="s">
         <v>15</v>
@@ -6027,7 +6027,7 @@
         <v>1</v>
       </c>
       <c r="D200" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E200" t="s">
         <v>15</v>
@@ -6047,7 +6047,7 @@
         <v>1</v>
       </c>
       <c r="D201" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E201" t="s">
         <v>15</v>
@@ -6067,7 +6067,7 @@
         <v>1</v>
       </c>
       <c r="D202" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E202" t="s">
         <v>15</v>
@@ -6087,7 +6087,7 @@
         <v>1</v>
       </c>
       <c r="D203" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="E203" t="s">
         <v>15</v>
@@ -6097,100 +6097,100 @@
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A204" t="s">
+      <c r="A204" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="B204" t="s">
-        <v>7</v>
-      </c>
-      <c r="C204">
-        <v>1</v>
+      <c r="B204" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C204" s="4">
+        <v>2</v>
       </c>
       <c r="D204" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E204" t="s">
         <v>15</v>
       </c>
       <c r="F204" t="s">
-        <v>416</v>
+        <v>469</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A205" t="s">
+      <c r="A205" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B205" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C205">
         <v>1</v>
       </c>
       <c r="D205" t="s">
-        <v>263</v>
-      </c>
-      <c r="E205" t="s">
-        <v>15</v>
+        <v>266</v>
       </c>
       <c r="F205" t="s">
         <v>416</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A206" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="B206" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C206" s="4">
-        <v>2</v>
-      </c>
-      <c r="D206" t="s">
-        <v>264</v>
-      </c>
-      <c r="E206" t="s">
-        <v>15</v>
-      </c>
-      <c r="F206" t="s">
-        <v>469</v>
+      <c r="A206" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C206" s="3">
+        <v>1</v>
+      </c>
+      <c r="D206" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="E206" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F206" s="3" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A207" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="B207" s="4" t="s">
+      <c r="A207" t="s">
+        <v>267</v>
+      </c>
+      <c r="B207" t="s">
         <v>7</v>
       </c>
       <c r="C207">
         <v>1</v>
       </c>
       <c r="D207" t="s">
-        <v>266</v>
+        <v>269</v>
+      </c>
+      <c r="E207" t="s">
+        <v>15</v>
       </c>
       <c r="F207" t="s">
         <v>416</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A208" s="3" t="s">
+      <c r="A208" t="s">
         <v>267</v>
       </c>
-      <c r="B208" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C208" s="3">
-        <v>1</v>
-      </c>
-      <c r="D208" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="E208" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F208" s="3" t="s">
-        <v>427</v>
+      <c r="B208" t="s">
+        <v>7</v>
+      </c>
+      <c r="C208">
+        <v>1</v>
+      </c>
+      <c r="D208" t="s">
+        <v>270</v>
+      </c>
+      <c r="E208" t="s">
+        <v>15</v>
+      </c>
+      <c r="F208" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.3">
@@ -6204,7 +6204,7 @@
         <v>1</v>
       </c>
       <c r="D209" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="E209" t="s">
         <v>15</v>
@@ -6224,7 +6224,7 @@
         <v>1</v>
       </c>
       <c r="D210" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="E210" t="s">
         <v>15</v>
@@ -6244,7 +6244,7 @@
         <v>1</v>
       </c>
       <c r="D211" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="E211" t="s">
         <v>15</v>
@@ -6264,7 +6264,7 @@
         <v>1</v>
       </c>
       <c r="D212" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="E212" t="s">
         <v>15</v>
@@ -6274,19 +6274,19 @@
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A213" t="s">
+      <c r="A213" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="B213" t="s">
-        <v>7</v>
-      </c>
-      <c r="C213">
-        <v>1</v>
-      </c>
-      <c r="D213" t="s">
-        <v>273</v>
-      </c>
-      <c r="E213" t="s">
+      <c r="B213" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C213" s="3">
+        <v>1</v>
+      </c>
+      <c r="D213" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="E213" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F213" t="s">
@@ -6304,7 +6304,7 @@
         <v>1</v>
       </c>
       <c r="D214" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="E214" t="s">
         <v>15</v>
@@ -6314,19 +6314,19 @@
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A215" s="3" t="s">
+      <c r="A215" t="s">
         <v>267</v>
       </c>
-      <c r="B215" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C215" s="3">
-        <v>1</v>
-      </c>
-      <c r="D215" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="E215" s="3" t="s">
+      <c r="B215" t="s">
+        <v>7</v>
+      </c>
+      <c r="C215">
+        <v>1</v>
+      </c>
+      <c r="D215" t="s">
+        <v>277</v>
+      </c>
+      <c r="E215" t="s">
         <v>15</v>
       </c>
       <c r="F215" t="s">
@@ -6344,7 +6344,7 @@
         <v>1</v>
       </c>
       <c r="D216" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="E216" t="s">
         <v>15</v>
@@ -6364,7 +6364,7 @@
         <v>1</v>
       </c>
       <c r="D217" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="E217" t="s">
         <v>15</v>
@@ -6384,7 +6384,7 @@
         <v>1</v>
       </c>
       <c r="D218" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E218" t="s">
         <v>15</v>
@@ -6400,11 +6400,8 @@
       <c r="B219" t="s">
         <v>7</v>
       </c>
-      <c r="C219">
-        <v>1</v>
-      </c>
       <c r="D219" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="E219" t="s">
         <v>15</v>
@@ -6414,59 +6411,62 @@
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A220" t="s">
-        <v>267</v>
-      </c>
-      <c r="B220" t="s">
-        <v>7</v>
-      </c>
-      <c r="C220">
-        <v>1</v>
-      </c>
-      <c r="D220" t="s">
-        <v>280</v>
-      </c>
-      <c r="E220" t="s">
-        <v>15</v>
-      </c>
-      <c r="F220" t="s">
-        <v>416</v>
+      <c r="A220" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B220" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C220" s="3">
+        <v>1</v>
+      </c>
+      <c r="D220" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="E220" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F220" s="3" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>267</v>
+        <v>282</v>
       </c>
       <c r="B221" t="s">
         <v>7</v>
       </c>
+      <c r="C221">
+        <v>1</v>
+      </c>
       <c r="D221" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="E221" t="s">
         <v>15</v>
       </c>
       <c r="F221" t="s">
-        <v>416</v>
+        <v>427</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A222" s="3" t="s">
+      <c r="A222" t="s">
         <v>282</v>
       </c>
-      <c r="B222" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C222" s="3">
-        <v>1</v>
-      </c>
-      <c r="D222" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="E222" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F222" s="3" t="s">
+      <c r="B222" t="s">
+        <v>7</v>
+      </c>
+      <c r="C222">
+        <v>1</v>
+      </c>
+      <c r="D222" t="s">
+        <v>285</v>
+      </c>
+      <c r="E222" t="s">
+        <v>15</v>
+      </c>
+      <c r="F222" t="s">
         <v>427</v>
       </c>
     </row>
@@ -6481,7 +6481,7 @@
         <v>1</v>
       </c>
       <c r="D223" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="E223" t="s">
         <v>15</v>
@@ -6491,23 +6491,23 @@
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A224" t="s">
+      <c r="A224" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="B224" t="s">
-        <v>7</v>
-      </c>
-      <c r="C224">
-        <v>1</v>
-      </c>
-      <c r="D224" t="s">
-        <v>285</v>
-      </c>
-      <c r="E224" t="s">
-        <v>15</v>
-      </c>
-      <c r="F224" t="s">
-        <v>427</v>
+      <c r="B224" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C224" s="3">
+        <v>2</v>
+      </c>
+      <c r="D224" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="E224" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F224" s="3" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.3">
@@ -6518,35 +6518,35 @@
         <v>7</v>
       </c>
       <c r="C225">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D225" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E225" t="s">
         <v>15</v>
       </c>
       <c r="F225" t="s">
-        <v>427</v>
+        <v>469</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A226" s="3" t="s">
+      <c r="A226" t="s">
         <v>282</v>
       </c>
-      <c r="B226" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C226" s="3">
-        <v>2</v>
-      </c>
-      <c r="D226" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="E226" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F226" s="3" t="s">
+      <c r="B226" t="s">
+        <v>7</v>
+      </c>
+      <c r="C226">
+        <v>2</v>
+      </c>
+      <c r="D226" t="s">
+        <v>288</v>
+      </c>
+      <c r="E226" t="s">
+        <v>15</v>
+      </c>
+      <c r="F226" t="s">
         <v>469</v>
       </c>
     </row>
@@ -6560,8 +6560,8 @@
       <c r="C227">
         <v>2</v>
       </c>
-      <c r="D227" t="s">
-        <v>287</v>
+      <c r="D227" s="5" t="s">
+        <v>289</v>
       </c>
       <c r="E227" t="s">
         <v>15</v>
@@ -6572,47 +6572,47 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="B228" t="s">
         <v>7</v>
       </c>
       <c r="C228">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D228" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="E228" t="s">
         <v>15</v>
       </c>
       <c r="F228" t="s">
-        <v>469</v>
+        <v>427</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="B229" t="s">
         <v>7</v>
       </c>
       <c r="C229">
-        <v>2</v>
-      </c>
-      <c r="D229" s="5" t="s">
-        <v>289</v>
+        <v>1</v>
+      </c>
+      <c r="D229" t="s">
+        <v>292</v>
       </c>
       <c r="E229" t="s">
         <v>15</v>
       </c>
       <c r="F229" t="s">
-        <v>469</v>
+        <v>427</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B230" t="s">
         <v>7</v>
@@ -6621,18 +6621,18 @@
         <v>1</v>
       </c>
       <c r="D230" t="s">
-        <v>291</v>
+        <v>42</v>
       </c>
       <c r="E230" t="s">
         <v>15</v>
       </c>
       <c r="F230" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="B231" t="s">
         <v>7</v>
@@ -6641,18 +6641,18 @@
         <v>1</v>
       </c>
       <c r="D231" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="E231" t="s">
         <v>15</v>
       </c>
       <c r="F231" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B232" t="s">
         <v>7</v>
@@ -6661,7 +6661,7 @@
         <v>1</v>
       </c>
       <c r="D232" t="s">
-        <v>42</v>
+        <v>296</v>
       </c>
       <c r="E232" t="s">
         <v>15</v>
@@ -6681,7 +6681,7 @@
         <v>1</v>
       </c>
       <c r="D233" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="E233" t="s">
         <v>15</v>
@@ -6701,7 +6701,7 @@
         <v>1</v>
       </c>
       <c r="D234" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E234" t="s">
         <v>15</v>
@@ -6718,16 +6718,16 @@
         <v>7</v>
       </c>
       <c r="C235">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D235" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="E235" t="s">
         <v>15</v>
       </c>
       <c r="F235" t="s">
-        <v>416</v>
+        <v>469</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.3">
@@ -6738,61 +6738,61 @@
         <v>7</v>
       </c>
       <c r="C236">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D236" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="E236" t="s">
         <v>15</v>
       </c>
       <c r="F236" t="s">
-        <v>416</v>
+        <v>469</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="B237" t="s">
         <v>7</v>
       </c>
       <c r="C237">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D237" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="E237" t="s">
         <v>15</v>
       </c>
       <c r="F237" t="s">
-        <v>469</v>
+        <v>416</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="B238" t="s">
         <v>7</v>
       </c>
       <c r="C238">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D238" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="E238" t="s">
         <v>15</v>
       </c>
       <c r="F238" t="s">
-        <v>469</v>
+        <v>416</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B239" t="s">
         <v>7</v>
@@ -6801,7 +6801,7 @@
         <v>1</v>
       </c>
       <c r="D239" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="E239" t="s">
         <v>15</v>
@@ -6812,7 +6812,7 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B240" t="s">
         <v>7</v>
@@ -6821,7 +6821,7 @@
         <v>1</v>
       </c>
       <c r="D240" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="E240" t="s">
         <v>15</v>
@@ -6841,7 +6841,7 @@
         <v>1</v>
       </c>
       <c r="D241" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="E241" t="s">
         <v>15</v>
@@ -6861,7 +6861,7 @@
         <v>1</v>
       </c>
       <c r="D242" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="E242" t="s">
         <v>15</v>
@@ -6878,16 +6878,16 @@
         <v>7</v>
       </c>
       <c r="C243">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D243" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="E243" t="s">
         <v>15</v>
       </c>
       <c r="F243" t="s">
-        <v>416</v>
+        <v>469</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.3">
@@ -6898,16 +6898,16 @@
         <v>7</v>
       </c>
       <c r="C244">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D244" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="E244" t="s">
         <v>15</v>
       </c>
       <c r="F244" t="s">
-        <v>416</v>
+        <v>469</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.3">
@@ -6921,7 +6921,7 @@
         <v>2</v>
       </c>
       <c r="D245" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="E245" t="s">
         <v>15</v>
@@ -6931,62 +6931,62 @@
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A246" t="s">
-        <v>304</v>
-      </c>
-      <c r="B246" t="s">
-        <v>7</v>
-      </c>
-      <c r="C246">
-        <v>2</v>
-      </c>
-      <c r="D246" t="s">
-        <v>310</v>
-      </c>
-      <c r="E246" t="s">
-        <v>15</v>
-      </c>
-      <c r="F246" t="s">
-        <v>469</v>
+      <c r="A246" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="B246" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C246" s="3">
+        <v>1</v>
+      </c>
+      <c r="D246" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="E246" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F246" s="3" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="B247" t="s">
         <v>7</v>
       </c>
       <c r="C247">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D247" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E247" t="s">
         <v>15</v>
       </c>
       <c r="F247" t="s">
-        <v>469</v>
+        <v>416</v>
       </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A248" s="3" t="s">
+      <c r="A248" t="s">
         <v>312</v>
       </c>
-      <c r="B248" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C248" s="3">
-        <v>1</v>
-      </c>
-      <c r="D248" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="E248" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F248" s="3" t="s">
+      <c r="B248" t="s">
+        <v>7</v>
+      </c>
+      <c r="C248">
+        <v>1</v>
+      </c>
+      <c r="D248" t="s">
+        <v>315</v>
+      </c>
+      <c r="E248" t="s">
+        <v>15</v>
+      </c>
+      <c r="F248" t="s">
         <v>416</v>
       </c>
     </row>
@@ -7001,7 +7001,7 @@
         <v>1</v>
       </c>
       <c r="D249" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="E249" t="s">
         <v>15</v>
@@ -7021,7 +7021,7 @@
         <v>1</v>
       </c>
       <c r="D250" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E250" t="s">
         <v>15</v>
@@ -7041,7 +7041,7 @@
         <v>1</v>
       </c>
       <c r="D251" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="E251" t="s">
         <v>15</v>
@@ -7061,7 +7061,7 @@
         <v>1</v>
       </c>
       <c r="D252" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E252" t="s">
         <v>15</v>
@@ -7081,7 +7081,7 @@
         <v>1</v>
       </c>
       <c r="D253" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="E253" t="s">
         <v>15</v>
@@ -7092,42 +7092,42 @@
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
       <c r="B254" t="s">
         <v>7</v>
       </c>
       <c r="C254">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D254" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="E254" t="s">
         <v>15</v>
       </c>
       <c r="F254" t="s">
-        <v>416</v>
+        <v>469</v>
       </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
       <c r="B255" t="s">
         <v>7</v>
       </c>
       <c r="C255">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D255" t="s">
-        <v>320</v>
+        <v>473</v>
       </c>
       <c r="E255" t="s">
         <v>15</v>
       </c>
       <c r="F255" t="s">
-        <v>416</v>
+        <v>469</v>
       </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.3">
@@ -7141,13 +7141,13 @@
         <v>2</v>
       </c>
       <c r="D256" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E256" t="s">
         <v>15</v>
       </c>
       <c r="F256" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.3">
@@ -7161,18 +7161,18 @@
         <v>2</v>
       </c>
       <c r="D257" t="s">
-        <v>473</v>
+        <v>350</v>
       </c>
       <c r="E257" t="s">
         <v>15</v>
       </c>
       <c r="F257" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="B258" t="s">
         <v>7</v>
@@ -7181,18 +7181,18 @@
         <v>2</v>
       </c>
       <c r="D258" t="s">
-        <v>323</v>
+        <v>476</v>
       </c>
       <c r="E258" t="s">
         <v>15</v>
       </c>
       <c r="F258" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>321</v>
+        <v>74</v>
       </c>
       <c r="B259" t="s">
         <v>7</v>
@@ -7201,18 +7201,18 @@
         <v>2</v>
       </c>
       <c r="D259" t="s">
-        <v>350</v>
+        <v>326</v>
       </c>
       <c r="E259" t="s">
         <v>15</v>
       </c>
       <c r="F259" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>324</v>
+        <v>74</v>
       </c>
       <c r="B260" t="s">
         <v>7</v>
@@ -7221,7 +7221,7 @@
         <v>2</v>
       </c>
       <c r="D260" t="s">
-        <v>476</v>
+        <v>327</v>
       </c>
       <c r="E260" t="s">
         <v>15</v>
@@ -7241,7 +7241,7 @@
         <v>2</v>
       </c>
       <c r="D261" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="E261" t="s">
         <v>15</v>
@@ -7261,7 +7261,7 @@
         <v>2</v>
       </c>
       <c r="D262" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="E262" t="s">
         <v>15</v>
@@ -7281,7 +7281,7 @@
         <v>2</v>
       </c>
       <c r="D263" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="E263" t="s">
         <v>15</v>
@@ -7301,7 +7301,7 @@
         <v>2</v>
       </c>
       <c r="D264" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="E264" t="s">
         <v>15</v>
@@ -7321,7 +7321,7 @@
         <v>2</v>
       </c>
       <c r="D265" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="E265" t="s">
         <v>15</v>
@@ -7341,7 +7341,7 @@
         <v>2</v>
       </c>
       <c r="D266" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="E266" t="s">
         <v>15</v>
@@ -7361,7 +7361,7 @@
         <v>2</v>
       </c>
       <c r="D267" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="E267" t="s">
         <v>15</v>
@@ -7381,7 +7381,7 @@
         <v>2</v>
       </c>
       <c r="D268" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="E268" t="s">
         <v>15</v>
@@ -7401,7 +7401,7 @@
         <v>2</v>
       </c>
       <c r="D269" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="E269" t="s">
         <v>15</v>
@@ -7421,7 +7421,7 @@
         <v>2</v>
       </c>
       <c r="D270" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="E270" t="s">
         <v>15</v>
@@ -7441,7 +7441,7 @@
         <v>2</v>
       </c>
       <c r="D271" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="E271" t="s">
         <v>15</v>
@@ -7461,7 +7461,7 @@
         <v>2</v>
       </c>
       <c r="D272" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E272" t="s">
         <v>15</v>
@@ -7470,7 +7470,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>74</v>
       </c>
@@ -7481,7 +7481,7 @@
         <v>2</v>
       </c>
       <c r="D273" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="E273" t="s">
         <v>15</v>
@@ -7490,9 +7490,9 @@
         <v>469</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>74</v>
+        <v>341</v>
       </c>
       <c r="B274" t="s">
         <v>7</v>
@@ -7501,7 +7501,7 @@
         <v>2</v>
       </c>
       <c r="D274" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="E274" t="s">
         <v>15</v>
@@ -7510,9 +7510,9 @@
         <v>469</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>74</v>
+        <v>341</v>
       </c>
       <c r="B275" t="s">
         <v>7</v>
@@ -7521,7 +7521,7 @@
         <v>2</v>
       </c>
       <c r="D275" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="E275" t="s">
         <v>15</v>
@@ -7530,9 +7530,9 @@
         <v>469</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="B276" t="s">
         <v>7</v>
@@ -7541,7 +7541,7 @@
         <v>2</v>
       </c>
       <c r="D276" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="E276" t="s">
         <v>15</v>
@@ -7550,9 +7550,9 @@
         <v>469</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="B277" t="s">
         <v>7</v>
@@ -7561,7 +7561,7 @@
         <v>2</v>
       </c>
       <c r="D277" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="E277" t="s">
         <v>15</v>
@@ -7570,9 +7570,9 @@
         <v>469</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>344</v>
+        <v>321</v>
       </c>
       <c r="B278" t="s">
         <v>7</v>
@@ -7581,7 +7581,7 @@
         <v>2</v>
       </c>
       <c r="D278" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="E278" t="s">
         <v>15</v>
@@ -7590,9 +7590,9 @@
         <v>469</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>344</v>
+        <v>321</v>
       </c>
       <c r="B279" t="s">
         <v>7</v>
@@ -7601,7 +7601,7 @@
         <v>2</v>
       </c>
       <c r="D279" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="E279" t="s">
         <v>15</v>
@@ -7610,7 +7610,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>321</v>
       </c>
@@ -7621,7 +7621,7 @@
         <v>2</v>
       </c>
       <c r="D280" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="E280" t="s">
         <v>15</v>
@@ -7630,7 +7630,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>321</v>
       </c>
@@ -7641,7 +7641,7 @@
         <v>2</v>
       </c>
       <c r="D281" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="E281" t="s">
         <v>15</v>
@@ -7650,7 +7650,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>321</v>
       </c>
@@ -7661,7 +7661,7 @@
         <v>2</v>
       </c>
       <c r="D282" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="E282" t="s">
         <v>15</v>
@@ -7670,7 +7670,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>321</v>
       </c>
@@ -7681,7 +7681,7 @@
         <v>2</v>
       </c>
       <c r="D283" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E283" t="s">
         <v>15</v>
@@ -7690,7 +7690,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>321</v>
       </c>
@@ -7701,7 +7701,7 @@
         <v>2</v>
       </c>
       <c r="D284" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="E284" t="s">
         <v>15</v>
@@ -7710,9 +7710,9 @@
         <v>469</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>321</v>
+        <v>354</v>
       </c>
       <c r="B285" t="s">
         <v>7</v>
@@ -7721,7 +7721,7 @@
         <v>2</v>
       </c>
       <c r="D285" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="E285" t="s">
         <v>15</v>
@@ -7730,9 +7730,9 @@
         <v>469</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>321</v>
+        <v>354</v>
       </c>
       <c r="B286" t="s">
         <v>7</v>
@@ -7741,7 +7741,7 @@
         <v>2</v>
       </c>
       <c r="D286" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="E286" t="s">
         <v>15</v>
@@ -7750,9 +7750,9 @@
         <v>469</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B287" t="s">
         <v>7</v>
@@ -7761,7 +7761,7 @@
         <v>2</v>
       </c>
       <c r="D287" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="E287" t="s">
         <v>15</v>
@@ -7770,90 +7770,90 @@
         <v>469</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A288" t="s">
-        <v>354</v>
-      </c>
-      <c r="B288" t="s">
-        <v>7</v>
-      </c>
-      <c r="C288">
-        <v>2</v>
-      </c>
-      <c r="D288" t="s">
-        <v>356</v>
-      </c>
-      <c r="E288" t="s">
-        <v>15</v>
-      </c>
-      <c r="F288" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A289" t="s">
-        <v>357</v>
-      </c>
-      <c r="B289" t="s">
-        <v>7</v>
-      </c>
-      <c r="C289">
-        <v>2</v>
-      </c>
-      <c r="D289" t="s">
-        <v>358</v>
-      </c>
-      <c r="E289" t="s">
-        <v>15</v>
-      </c>
-      <c r="F289" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="290" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A290" s="6" t="s">
+    <row r="288" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A288" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="B290" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C290" s="6">
-        <v>1</v>
-      </c>
-      <c r="D290" s="6" t="s">
+      <c r="B288" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C288" s="6">
+        <v>1</v>
+      </c>
+      <c r="D288" s="6" t="s">
         <v>360</v>
       </c>
-      <c r="E290" s="6" t="s">
+      <c r="E288" s="6" t="s">
         <v>361</v>
       </c>
-      <c r="F290" s="6" t="s">
+      <c r="F288" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G290" t="s">
+      <c r="G288" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A291" s="6" t="s">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A289" s="6" t="s">
         <v>362</v>
       </c>
-      <c r="B291" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C291" s="6">
-        <v>1</v>
-      </c>
-      <c r="D291" s="6" t="s">
+      <c r="B289" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C289" s="6">
+        <v>1</v>
+      </c>
+      <c r="D289" s="6" t="s">
         <v>415</v>
       </c>
-      <c r="E291" s="6" t="s">
+      <c r="E289" s="6" t="s">
         <v>361</v>
       </c>
-      <c r="F291" s="6" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F289" s="6" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A290" t="s">
+        <v>363</v>
+      </c>
+      <c r="B290" t="s">
+        <v>7</v>
+      </c>
+      <c r="C290">
+        <v>1</v>
+      </c>
+      <c r="D290" t="s">
+        <v>364</v>
+      </c>
+      <c r="E290" t="s">
+        <v>265</v>
+      </c>
+      <c r="F290" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A291" t="s">
+        <v>363</v>
+      </c>
+      <c r="B291" t="s">
+        <v>7</v>
+      </c>
+      <c r="C291">
+        <v>1</v>
+      </c>
+      <c r="D291" t="s">
+        <v>365</v>
+      </c>
+      <c r="E291" t="s">
+        <v>366</v>
+      </c>
+      <c r="F291" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>363</v>
       </c>
@@ -7863,17 +7863,17 @@
       <c r="C292">
         <v>1</v>
       </c>
-      <c r="D292" t="s">
-        <v>364</v>
+      <c r="D292" s="7" t="s">
+        <v>430</v>
       </c>
       <c r="E292" t="s">
-        <v>265</v>
+        <v>15</v>
       </c>
       <c r="F292" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>363</v>
       </c>
@@ -7883,19 +7883,19 @@
       <c r="C293">
         <v>1</v>
       </c>
-      <c r="D293" t="s">
-        <v>365</v>
+      <c r="D293" s="7" t="s">
+        <v>431</v>
       </c>
       <c r="E293" t="s">
-        <v>366</v>
+        <v>15</v>
       </c>
       <c r="F293" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="B294" t="s">
         <v>7</v>
@@ -7903,8 +7903,8 @@
       <c r="C294">
         <v>1</v>
       </c>
-      <c r="D294" s="7" t="s">
-        <v>430</v>
+      <c r="D294" t="s">
+        <v>370</v>
       </c>
       <c r="E294" t="s">
         <v>15</v>
@@ -7913,9 +7913,9 @@
         <v>416</v>
       </c>
     </row>
-    <row r="295" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="B295" t="s">
         <v>7</v>
@@ -7923,8 +7923,8 @@
       <c r="C295">
         <v>1</v>
       </c>
-      <c r="D295" s="7" t="s">
-        <v>431</v>
+      <c r="D295" t="s">
+        <v>371</v>
       </c>
       <c r="E295" t="s">
         <v>15</v>
@@ -7933,7 +7933,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="296" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>369</v>
       </c>
@@ -7944,7 +7944,7 @@
         <v>1</v>
       </c>
       <c r="D296" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="E296" t="s">
         <v>15</v>
@@ -7953,7 +7953,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="297" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>369</v>
       </c>
@@ -7964,7 +7964,7 @@
         <v>1</v>
       </c>
       <c r="D297" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="E297" t="s">
         <v>15</v>
@@ -7973,7 +7973,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="298" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>369</v>
       </c>
@@ -7984,7 +7984,7 @@
         <v>1</v>
       </c>
       <c r="D298" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="E298" t="s">
         <v>15</v>
@@ -7993,7 +7993,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="299" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>369</v>
       </c>
@@ -8004,7 +8004,7 @@
         <v>1</v>
       </c>
       <c r="D299" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="E299" t="s">
         <v>15</v>
@@ -8013,7 +8013,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="300" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>369</v>
       </c>
@@ -8024,7 +8024,7 @@
         <v>1</v>
       </c>
       <c r="D300" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="E300" t="s">
         <v>15</v>
@@ -8033,7 +8033,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="301" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>369</v>
       </c>
@@ -8044,7 +8044,7 @@
         <v>1</v>
       </c>
       <c r="D301" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="E301" t="s">
         <v>15</v>
@@ -8053,9 +8053,9 @@
         <v>416</v>
       </c>
     </row>
-    <row r="302" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
       <c r="B302" t="s">
         <v>7</v>
@@ -8064,7 +8064,7 @@
         <v>1</v>
       </c>
       <c r="D302" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="E302" t="s">
         <v>15</v>
@@ -8073,9 +8073,9 @@
         <v>416</v>
       </c>
     </row>
-    <row r="303" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
       <c r="B303" t="s">
         <v>7</v>
@@ -8084,7 +8084,7 @@
         <v>1</v>
       </c>
       <c r="D303" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="E303" t="s">
         <v>15</v>
@@ -8093,7 +8093,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="304" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>378</v>
       </c>
@@ -8104,7 +8104,7 @@
         <v>1</v>
       </c>
       <c r="D304" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="E304" t="s">
         <v>15</v>
@@ -8124,7 +8124,7 @@
         <v>1</v>
       </c>
       <c r="D305" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="E305" t="s">
         <v>15</v>
@@ -8144,7 +8144,7 @@
         <v>1</v>
       </c>
       <c r="D306" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="E306" t="s">
         <v>15</v>
@@ -8164,7 +8164,7 @@
         <v>1</v>
       </c>
       <c r="D307" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="E307" t="s">
         <v>15</v>
@@ -8184,7 +8184,7 @@
         <v>1</v>
       </c>
       <c r="D308" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="E308" t="s">
         <v>15</v>
@@ -8195,7 +8195,7 @@
     </row>
     <row r="309" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>378</v>
+        <v>386</v>
       </c>
       <c r="B309" t="s">
         <v>7</v>
@@ -8204,7 +8204,7 @@
         <v>1</v>
       </c>
       <c r="D309" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="E309" t="s">
         <v>15</v>
@@ -8215,7 +8215,7 @@
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>378</v>
+        <v>386</v>
       </c>
       <c r="B310" t="s">
         <v>7</v>
@@ -8224,7 +8224,7 @@
         <v>1</v>
       </c>
       <c r="D310" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="E310" t="s">
         <v>15</v>
@@ -8244,7 +8244,7 @@
         <v>1</v>
       </c>
       <c r="D311" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="E311" t="s">
         <v>15</v>
@@ -8264,7 +8264,7 @@
         <v>1</v>
       </c>
       <c r="D312" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="E312" t="s">
         <v>15</v>
@@ -8284,7 +8284,7 @@
         <v>1</v>
       </c>
       <c r="D313" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="E313" t="s">
         <v>15</v>
@@ -8304,7 +8304,7 @@
         <v>1</v>
       </c>
       <c r="D314" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="E314" t="s">
         <v>15</v>
@@ -8324,7 +8324,7 @@
         <v>1</v>
       </c>
       <c r="D315" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="E315" t="s">
         <v>15</v>
@@ -8335,7 +8335,7 @@
     </row>
     <row r="316" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>386</v>
+        <v>394</v>
       </c>
       <c r="B316" t="s">
         <v>7</v>
@@ -8344,7 +8344,7 @@
         <v>1</v>
       </c>
       <c r="D316" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="E316" t="s">
         <v>15</v>
@@ -8355,7 +8355,7 @@
     </row>
     <row r="317" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>386</v>
+        <v>394</v>
       </c>
       <c r="B317" t="s">
         <v>7</v>
@@ -8364,7 +8364,7 @@
         <v>1</v>
       </c>
       <c r="D317" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="E317" t="s">
         <v>15</v>
@@ -8384,7 +8384,7 @@
         <v>1</v>
       </c>
       <c r="D318" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="E318" t="s">
         <v>15</v>
@@ -8403,8 +8403,8 @@
       <c r="C319">
         <v>1</v>
       </c>
-      <c r="D319" t="s">
-        <v>396</v>
+      <c r="D319" s="8" t="s">
+        <v>398</v>
       </c>
       <c r="E319" t="s">
         <v>15</v>
@@ -8424,7 +8424,7 @@
         <v>1</v>
       </c>
       <c r="D320" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="E320" t="s">
         <v>15</v>
@@ -8443,8 +8443,8 @@
       <c r="C321">
         <v>1</v>
       </c>
-      <c r="D321" s="8" t="s">
-        <v>398</v>
+      <c r="D321" t="s">
+        <v>400</v>
       </c>
       <c r="E321" t="s">
         <v>15</v>
@@ -8464,7 +8464,7 @@
         <v>1</v>
       </c>
       <c r="D322" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="E322" t="s">
         <v>15</v>
@@ -8484,7 +8484,7 @@
         <v>1</v>
       </c>
       <c r="D323" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="E323" t="s">
         <v>15</v>
@@ -8504,7 +8504,7 @@
         <v>1</v>
       </c>
       <c r="D324" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="E324" t="s">
         <v>15</v>
@@ -8524,7 +8524,7 @@
         <v>1</v>
       </c>
       <c r="D325" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="E325" t="s">
         <v>15</v>
@@ -8544,7 +8544,7 @@
         <v>1</v>
       </c>
       <c r="D326" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="E326" t="s">
         <v>15</v>
@@ -8564,7 +8564,7 @@
         <v>1</v>
       </c>
       <c r="D327" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="E327" t="s">
         <v>15</v>
@@ -8584,7 +8584,7 @@
         <v>1</v>
       </c>
       <c r="D328" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="E328" t="s">
         <v>15</v>
@@ -8604,7 +8604,7 @@
         <v>1</v>
       </c>
       <c r="D329" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="E329" t="s">
         <v>15</v>
@@ -8624,7 +8624,7 @@
         <v>1</v>
       </c>
       <c r="D330" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="E330" t="s">
         <v>15</v>
@@ -8644,7 +8644,7 @@
         <v>1</v>
       </c>
       <c r="D331" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="E331" t="s">
         <v>15</v>
@@ -8664,7 +8664,7 @@
         <v>1</v>
       </c>
       <c r="D332" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="E332" t="s">
         <v>15</v>
@@ -8681,16 +8681,16 @@
         <v>7</v>
       </c>
       <c r="C333">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D333" t="s">
-        <v>410</v>
+        <v>474</v>
       </c>
       <c r="E333" t="s">
         <v>15</v>
       </c>
       <c r="F333" t="s">
-        <v>416</v>
+        <v>469</v>
       </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.3">
@@ -8701,41 +8701,41 @@
         <v>7</v>
       </c>
       <c r="C334">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D334" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E334" t="s">
         <v>15</v>
       </c>
       <c r="F334" t="s">
-        <v>416</v>
+        <v>469</v>
       </c>
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
-        <v>394</v>
+        <v>413</v>
       </c>
       <c r="B335" t="s">
         <v>7</v>
       </c>
       <c r="C335">
-        <v>2</v>
-      </c>
-      <c r="D335" t="s">
-        <v>474</v>
+        <v>1</v>
+      </c>
+      <c r="D335" s="1" t="s">
+        <v>291</v>
       </c>
       <c r="E335" t="s">
         <v>15</v>
       </c>
       <c r="F335" t="s">
-        <v>469</v>
+        <v>416</v>
       </c>
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
-        <v>394</v>
+        <v>477</v>
       </c>
       <c r="B336" t="s">
         <v>7</v>
@@ -8744,27 +8744,27 @@
         <v>2</v>
       </c>
       <c r="D336" t="s">
-        <v>412</v>
+        <v>479</v>
       </c>
       <c r="E336" t="s">
         <v>15</v>
       </c>
       <c r="F336" t="s">
-        <v>469</v>
+        <v>416</v>
       </c>
     </row>
     <row r="337" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
-        <v>413</v>
+        <v>477</v>
       </c>
       <c r="B337" t="s">
         <v>7</v>
       </c>
       <c r="C337">
-        <v>1</v>
-      </c>
-      <c r="D337" s="1" t="s">
-        <v>291</v>
+        <v>2</v>
+      </c>
+      <c r="D337" t="s">
+        <v>480</v>
       </c>
       <c r="E337" t="s">
         <v>15</v>
@@ -8784,7 +8784,7 @@
         <v>2</v>
       </c>
       <c r="D338" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="E338" t="s">
         <v>15</v>
@@ -8804,7 +8804,7 @@
         <v>2</v>
       </c>
       <c r="D339" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="E339" t="s">
         <v>15</v>
@@ -8824,7 +8824,7 @@
         <v>2</v>
       </c>
       <c r="D340" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="E340" t="s">
         <v>15</v>
@@ -8844,7 +8844,7 @@
         <v>2</v>
       </c>
       <c r="D341" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="E341" t="s">
         <v>15</v>
@@ -8864,7 +8864,7 @@
         <v>2</v>
       </c>
       <c r="D342" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="E342" t="s">
         <v>15</v>
@@ -8884,7 +8884,7 @@
         <v>2</v>
       </c>
       <c r="D343" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="E343" t="s">
         <v>15</v>
@@ -8904,52 +8904,12 @@
         <v>2</v>
       </c>
       <c r="D344" t="s">
-        <v>485</v>
+        <v>472</v>
       </c>
       <c r="E344" t="s">
         <v>15</v>
       </c>
       <c r="F344" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A345" t="s">
-        <v>477</v>
-      </c>
-      <c r="B345" t="s">
-        <v>7</v>
-      </c>
-      <c r="C345">
-        <v>2</v>
-      </c>
-      <c r="D345" t="s">
-        <v>486</v>
-      </c>
-      <c r="E345" t="s">
-        <v>15</v>
-      </c>
-      <c r="F345" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A346" t="s">
-        <v>477</v>
-      </c>
-      <c r="B346" t="s">
-        <v>7</v>
-      </c>
-      <c r="C346">
-        <v>2</v>
-      </c>
-      <c r="D346" t="s">
-        <v>472</v>
-      </c>
-      <c r="E346" t="s">
-        <v>15</v>
-      </c>
-      <c r="F346" t="s">
         <v>416</v>
       </c>
     </row>

</xml_diff>